<commit_message>
State vector inclusions and normalization changes
Added a single dimension to the state vector for each player, the sum of the player purchased cards.  Changed normalization for many dimensions, moving to normalize gold separately.  Cards are also normalized to 10 to try to align all with what they actually do - cards being equivalent to gems as far as purchase math goes.
</commit_message>
<xml_diff>
--- a/Splendor/Environment/Splendor_components/Board_components/Splendor_cards_numeric.xlsx
+++ b/Splendor/Environment/Splendor_components/Board_components/Splendor_cards_numeric.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Python_Files\Splendor\Environment\Splendor_components\Board_components\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Coding Programs\GitHub\Splendor-AI\Splendor\Environment\Splendor_components\Board_components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FC828D-50C6-41B5-AD0B-A6D1920506C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013B3419-C3FC-45ED-8648-B15DB2C68348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19455" yWindow="2115" windowWidth="15120" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26340" yWindow="3450" windowWidth="18090" windowHeight="15885" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0" sheetId="1" r:id="rId1"/>
     <sheet name="1" sheetId="3" r:id="rId2"/>
     <sheet name="2" sheetId="4" r:id="rId3"/>
-    <sheet name="3" sheetId="5" r:id="rId4"/>
+    <sheet name="Noble" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'0'!$B$1:$I$45</definedName>
@@ -378,7 +378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -2835,7 +2835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5EFF4C-5A62-4F84-A501-5E8E8E55D25C}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Added dueling heads and fixed bug in cards data
</commit_message>
<xml_diff>
--- a/Splendor/Environment/Splendor_components/Board_components/Splendor_cards_numeric.xlsx
+++ b/Splendor/Environment/Splendor_components/Board_components/Splendor_cards_numeric.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Coding Programs\GitHub\Splendor-AI\Splendor\Environment\Splendor_components\Board_components\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\Splendor-AI\Splendor\Environment\Splendor_components\Board_components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013B3419-C3FC-45ED-8648-B15DB2C68348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338915C8-5A92-4E30-9E77-57D60C94FCFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26340" yWindow="3450" windowWidth="18090" windowHeight="15885" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17175" yWindow="4005" windowWidth="19215" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Noble" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'0'!$B$1:$I$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'0'!$A$1:$H$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,6 +36,9 @@
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -378,7 +381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -2835,7 +2838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5EFF4C-5A62-4F84-A501-5E8E8E55D25C}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>